<commit_message>
Scrum Master - 2 Hari 1
</commit_message>
<xml_diff>
--- a/Burntdown Chart.xlsx
+++ b/Burntdown Chart.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hasan\Desktop\Project TKPL\Projek TKKPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jackyson\Desktop\Projek TKKPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="32">
   <si>
     <t>Kegiatan</t>
   </si>
@@ -115,6 +115,12 @@
   <si>
     <t>HARI 11</t>
   </si>
+  <si>
+    <t>HARI 12</t>
+  </si>
+  <si>
+    <t>EDIT TAMPILAN</t>
+  </si>
 </sst>
 </file>
 
@@ -166,7 +172,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -198,11 +204,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -229,6 +272,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -352,11 +404,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1249522608"/>
-        <c:axId val="-1249529136"/>
+        <c:axId val="830789424"/>
+        <c:axId val="830789968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1249522608"/>
+        <c:axId val="830789424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -398,7 +450,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1249529136"/>
+        <c:crossAx val="830789968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -406,7 +458,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1249529136"/>
+        <c:axId val="830789968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -457,7 +509,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1249522608"/>
+        <c:crossAx val="830789424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -551,6 +603,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -652,11 +705,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1251072976"/>
-        <c:axId val="-1251073520"/>
+        <c:axId val="835286032"/>
+        <c:axId val="835287120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1251072976"/>
+        <c:axId val="835286032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -699,7 +752,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1251073520"/>
+        <c:crossAx val="835287120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -707,7 +760,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1251073520"/>
+        <c:axId val="835287120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -758,7 +811,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1251072976"/>
+        <c:crossAx val="835286032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -852,6 +905,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -943,11 +997,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1251079504"/>
-        <c:axId val="-1251080048"/>
+        <c:axId val="835289296"/>
+        <c:axId val="835502992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1251079504"/>
+        <c:axId val="835289296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -990,7 +1044,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1251080048"/>
+        <c:crossAx val="835502992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -998,7 +1052,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1251080048"/>
+        <c:axId val="835502992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1049,7 +1103,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1251079504"/>
+        <c:crossAx val="835289296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1245,11 +1299,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1251086032"/>
-        <c:axId val="-1251085488"/>
+        <c:axId val="835517136"/>
+        <c:axId val="835506256"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1251086032"/>
+        <c:axId val="835517136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1292,7 +1346,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1251085488"/>
+        <c:crossAx val="835506256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1300,7 +1354,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1251085488"/>
+        <c:axId val="835506256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1351,7 +1405,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1251086032"/>
+        <c:crossAx val="835517136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1537,11 +1591,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1189230784"/>
-        <c:axId val="-1189223712"/>
+        <c:axId val="835515504"/>
+        <c:axId val="835513328"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1189230784"/>
+        <c:axId val="835515504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1584,7 +1638,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1189223712"/>
+        <c:crossAx val="835513328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1592,7 +1646,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1189223712"/>
+        <c:axId val="835513328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1643,7 +1697,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1189230784"/>
+        <c:crossAx val="835515504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1839,11 +1893,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1189236224"/>
-        <c:axId val="-1189230240"/>
+        <c:axId val="835504624"/>
+        <c:axId val="835516048"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1189236224"/>
+        <c:axId val="835504624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1886,7 +1940,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1189230240"/>
+        <c:crossAx val="835516048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1894,7 +1948,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1189230240"/>
+        <c:axId val="835516048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1945,7 +1999,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1189236224"/>
+        <c:crossAx val="835504624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2136,11 +2190,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1189236768"/>
-        <c:axId val="-1189224800"/>
+        <c:axId val="835512240"/>
+        <c:axId val="835513872"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1189236768"/>
+        <c:axId val="835512240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2183,7 +2237,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1189224800"/>
+        <c:crossAx val="835513872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2191,7 +2245,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1189224800"/>
+        <c:axId val="835513872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2242,7 +2296,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1189236768"/>
+        <c:crossAx val="835512240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2438,11 +2492,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1154897280"/>
-        <c:axId val="-1154898912"/>
+        <c:axId val="835509520"/>
+        <c:axId val="835507344"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1154897280"/>
+        <c:axId val="835509520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2485,7 +2539,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1154898912"/>
+        <c:crossAx val="835507344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2493,7 +2547,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1154898912"/>
+        <c:axId val="835507344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2544,7 +2598,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1154897280"/>
+        <c:crossAx val="835509520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2725,11 +2779,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1154000128"/>
-        <c:axId val="-1153990880"/>
+        <c:axId val="835507888"/>
+        <c:axId val="835514960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1154000128"/>
+        <c:axId val="835507888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2772,7 +2826,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1153990880"/>
+        <c:crossAx val="835514960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2780,7 +2834,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1153990880"/>
+        <c:axId val="835514960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2831,7 +2885,642 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1154000128"/>
+        <c:crossAx val="835507888"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="id-ID"/>
+              <a:t>Minggu</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="id-ID" baseline="0"/>
+              <a:t> 1</a:t>
+            </a:r>
+            <a:endParaRPr lang="id-ID"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.0025371828521436E-2"/>
+          <c:y val="0.17171296296296298"/>
+          <c:w val="0.9155301837270341"/>
+          <c:h val="0.72088764946048411"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$285:$I$285</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Senin</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Selasa</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Rabu</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Kamis</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Jumat</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sabtu</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Minggu</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$290:$I$290</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="788161264"/>
+        <c:axId val="788160176"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="788161264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="788160176"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="788160176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="788161264"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Minggu 2 - Senin -- Jumat</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$L$285:$P$285</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Senin</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Selasa</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Rabu</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Kamis</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Jumat</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$L$290:$P$290</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="879876192"/>
+        <c:axId val="879893056"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="879876192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="879893056"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="879893056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="879876192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2985,11 +3674,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1249530768"/>
-        <c:axId val="-1249519888"/>
+        <c:axId val="830779632"/>
+        <c:axId val="830785616"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1249530768"/>
+        <c:axId val="830779632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3031,7 +3720,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1249519888"/>
+        <c:crossAx val="830785616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -3039,7 +3728,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1249519888"/>
+        <c:axId val="830785616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3090,7 +3779,298 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1249530768"/>
+        <c:crossAx val="830779632"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Minggu 2 -</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Sabtu &amp; Minggu</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$S$285:$T$285</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Sabtu</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Minggu</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$S$290:$T$290</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="879900672"/>
+        <c:axId val="879901216"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="879900672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="879901216"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="879901216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="879900672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3330,11 +4310,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1249525328"/>
-        <c:axId val="-1249521520"/>
+        <c:axId val="830790512"/>
+        <c:axId val="830791056"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1249525328"/>
+        <c:axId val="830790512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3377,7 +4357,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1249521520"/>
+        <c:crossAx val="830791056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3385,7 +4365,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1249521520"/>
+        <c:axId val="830791056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3436,7 +4416,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1249525328"/>
+        <c:crossAx val="830790512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3600,11 +4580,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1249516624"/>
-        <c:axId val="-1249528592"/>
+        <c:axId val="835290384"/>
+        <c:axId val="835279504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1249516624"/>
+        <c:axId val="835290384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3647,7 +4627,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1249528592"/>
+        <c:crossAx val="835279504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3655,7 +4635,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1249528592"/>
+        <c:axId val="835279504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3706,7 +4686,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1249516624"/>
+        <c:crossAx val="835290384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3861,11 +4841,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1249524240"/>
-        <c:axId val="-1249523696"/>
+        <c:axId val="835283312"/>
+        <c:axId val="835280048"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1249524240"/>
+        <c:axId val="835283312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3908,7 +4888,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1249523696"/>
+        <c:crossAx val="835280048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3916,7 +4896,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1249523696"/>
+        <c:axId val="835280048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3967,7 +4947,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1249524240"/>
+        <c:crossAx val="835283312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4122,11 +5102,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1251075152"/>
-        <c:axId val="-1251083312"/>
+        <c:axId val="835282224"/>
+        <c:axId val="835277872"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1251075152"/>
+        <c:axId val="835282224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4169,7 +5149,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1251083312"/>
+        <c:crossAx val="835277872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4177,7 +5157,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1251083312"/>
+        <c:axId val="835277872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4228,7 +5208,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1251075152"/>
+        <c:crossAx val="835282224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4353,11 +5333,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1251077328"/>
-        <c:axId val="-1251084944"/>
+        <c:axId val="835291472"/>
+        <c:axId val="835287664"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1251077328"/>
+        <c:axId val="835291472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4400,7 +5380,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1251084944"/>
+        <c:crossAx val="835287664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4408,7 +5388,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1251084944"/>
+        <c:axId val="835287664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4459,7 +5439,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1251077328"/>
+        <c:crossAx val="835291472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4553,6 +5533,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4654,11 +5635,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1251074064"/>
-        <c:axId val="-1251086576"/>
+        <c:axId val="835284400"/>
+        <c:axId val="835284944"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1251074064"/>
+        <c:axId val="835284400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4701,7 +5682,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1251086576"/>
+        <c:crossAx val="835284944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4709,7 +5690,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1251086576"/>
+        <c:axId val="835284944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4760,7 +5741,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1251074064"/>
+        <c:crossAx val="835284400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4849,6 +5830,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4940,11 +5922,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1251076784"/>
-        <c:axId val="-1251081136"/>
+        <c:axId val="835276784"/>
+        <c:axId val="835277328"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1251076784"/>
+        <c:axId val="835276784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4987,7 +5969,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1251081136"/>
+        <c:crossAx val="835277328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4995,7 +5977,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1251081136"/>
+        <c:axId val="835277328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5046,7 +6028,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1251076784"/>
+        <c:crossAx val="835276784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5455,7 +6437,127 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors18.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors19.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors20.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -10419,7 +11521,1555 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style18.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style19.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style20.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -15071,6 +17721,98 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>291</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>305</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="19" name="Chart 18"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId18"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>156882</xdr:colOff>
+      <xdr:row>291</xdr:row>
+      <xdr:rowOff>23532</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>145677</xdr:colOff>
+      <xdr:row>305</xdr:row>
+      <xdr:rowOff>99732</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="22" name="Chart 21"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId19"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>515472</xdr:colOff>
+      <xdr:row>291</xdr:row>
+      <xdr:rowOff>1120</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>515472</xdr:colOff>
+      <xdr:row>305</xdr:row>
+      <xdr:rowOff>77320</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="23" name="Chart 22"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId20"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -15337,16 +18079,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R267"/>
+  <dimension ref="A1:T290"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A251" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q270" sqref="Q270"/>
+    <sheetView tabSelected="1" topLeftCell="A275" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T280" sqref="T280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16.5703125" customWidth="1"/>
     <col min="11" max="11" width="14.28515625" customWidth="1"/>
+    <col min="18" max="18" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:13" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17994,7 +20737,7 @@
     <row r="261" spans="1:18" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A261" s="6"/>
       <c r="B261" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C261" s="9"/>
       <c r="D261" s="9"/>
@@ -18338,8 +21081,377 @@
         <v>6</v>
       </c>
     </row>
+    <row r="284" spans="1:20" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A284" s="6"/>
+      <c r="B284" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C284" s="9"/>
+      <c r="D284" s="9"/>
+      <c r="E284" s="9"/>
+      <c r="F284" s="9"/>
+      <c r="G284" s="9"/>
+      <c r="H284" s="9"/>
+      <c r="I284" s="9"/>
+      <c r="J284" s="9"/>
+      <c r="K284" s="9"/>
+      <c r="L284" s="9"/>
+      <c r="M284" s="9"/>
+    </row>
+    <row r="285" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A285" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B285" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C285" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D285" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E285" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F285" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G285" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H285" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I285" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J285" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="K285" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L285" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M285" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N285" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O285" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P285" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="R285" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S285" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="T285" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="286" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A286" s="10"/>
+      <c r="B286" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C286" s="1">
+        <v>2</v>
+      </c>
+      <c r="D286" s="1">
+        <v>1</v>
+      </c>
+      <c r="E286" s="1">
+        <v>2</v>
+      </c>
+      <c r="F286" s="1">
+        <v>1</v>
+      </c>
+      <c r="G286" s="1">
+        <v>1</v>
+      </c>
+      <c r="H286" s="1">
+        <v>1</v>
+      </c>
+      <c r="I286" s="1">
+        <v>1</v>
+      </c>
+      <c r="J286" s="10"/>
+      <c r="K286" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L286" s="1">
+        <v>1</v>
+      </c>
+      <c r="M286" s="1">
+        <v>1</v>
+      </c>
+      <c r="N286" s="1">
+        <v>2</v>
+      </c>
+      <c r="O286" s="1">
+        <v>3</v>
+      </c>
+      <c r="P286" s="1">
+        <v>2</v>
+      </c>
+      <c r="R286" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="S286" s="1">
+        <v>2</v>
+      </c>
+      <c r="T286" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="287" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A287" s="10"/>
+      <c r="B287" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C287" s="1">
+        <v>2</v>
+      </c>
+      <c r="D287" s="1">
+        <v>1</v>
+      </c>
+      <c r="E287" s="1">
+        <v>1</v>
+      </c>
+      <c r="F287" s="1">
+        <v>1</v>
+      </c>
+      <c r="G287" s="1">
+        <v>2</v>
+      </c>
+      <c r="H287" s="1">
+        <v>2</v>
+      </c>
+      <c r="I287" s="1">
+        <v>2</v>
+      </c>
+      <c r="J287" s="10"/>
+      <c r="K287" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L287" s="1">
+        <v>1</v>
+      </c>
+      <c r="M287" s="1">
+        <v>2</v>
+      </c>
+      <c r="N287" s="1">
+        <v>2</v>
+      </c>
+      <c r="O287" s="1">
+        <v>2</v>
+      </c>
+      <c r="P287" s="1">
+        <v>2</v>
+      </c>
+      <c r="R287" s="12"/>
+      <c r="S287" s="1">
+        <v>3</v>
+      </c>
+      <c r="T287" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="288" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A288" s="10"/>
+      <c r="B288" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C288" s="1">
+        <v>2</v>
+      </c>
+      <c r="D288" s="1">
+        <v>1</v>
+      </c>
+      <c r="E288" s="1">
+        <v>1</v>
+      </c>
+      <c r="F288" s="1">
+        <v>2</v>
+      </c>
+      <c r="G288" s="1">
+        <v>2</v>
+      </c>
+      <c r="H288" s="1">
+        <v>1</v>
+      </c>
+      <c r="I288" s="1">
+        <v>2</v>
+      </c>
+      <c r="J288" s="10"/>
+      <c r="K288" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L288" s="1">
+        <v>1</v>
+      </c>
+      <c r="M288" s="1">
+        <v>1</v>
+      </c>
+      <c r="N288" s="1">
+        <v>1</v>
+      </c>
+      <c r="O288" s="1">
+        <v>2</v>
+      </c>
+      <c r="P288" s="1">
+        <v>2</v>
+      </c>
+      <c r="R288" s="12"/>
+      <c r="S288" s="1">
+        <v>3</v>
+      </c>
+      <c r="T288" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="289" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A289" s="10"/>
+      <c r="B289" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C289" s="1">
+        <v>2</v>
+      </c>
+      <c r="D289" s="1">
+        <v>1</v>
+      </c>
+      <c r="E289" s="1">
+        <v>1</v>
+      </c>
+      <c r="F289" s="1">
+        <v>1</v>
+      </c>
+      <c r="G289" s="1">
+        <v>1</v>
+      </c>
+      <c r="H289" s="1">
+        <v>1</v>
+      </c>
+      <c r="I289" s="1">
+        <v>1</v>
+      </c>
+      <c r="J289" s="10"/>
+      <c r="K289" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L289" s="1">
+        <v>1</v>
+      </c>
+      <c r="M289" s="1">
+        <v>1</v>
+      </c>
+      <c r="N289" s="1">
+        <v>2</v>
+      </c>
+      <c r="O289" s="1">
+        <v>3</v>
+      </c>
+      <c r="P289" s="1">
+        <v>2</v>
+      </c>
+      <c r="R289" s="13"/>
+      <c r="S289" s="1">
+        <v>3</v>
+      </c>
+      <c r="T289" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="290" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A290" s="10"/>
+      <c r="B290" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C290" s="1">
+        <f>SUM(C286:C289)</f>
+        <v>8</v>
+      </c>
+      <c r="D290" s="1">
+        <f>SUM(D286:D289)</f>
+        <v>4</v>
+      </c>
+      <c r="E290" s="1">
+        <f t="shared" ref="E290:I290" si="17">SUM(E286:E289)</f>
+        <v>5</v>
+      </c>
+      <c r="F290" s="1">
+        <f t="shared" si="17"/>
+        <v>5</v>
+      </c>
+      <c r="G290" s="1">
+        <f t="shared" si="17"/>
+        <v>6</v>
+      </c>
+      <c r="H290" s="1">
+        <f t="shared" si="17"/>
+        <v>5</v>
+      </c>
+      <c r="I290" s="1">
+        <f t="shared" si="17"/>
+        <v>6</v>
+      </c>
+      <c r="J290" s="10"/>
+      <c r="K290" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L290" s="1">
+        <f>SUM(L286:L289)</f>
+        <v>4</v>
+      </c>
+      <c r="M290" s="1">
+        <f>SUM(M286:M289)</f>
+        <v>5</v>
+      </c>
+      <c r="N290" s="1">
+        <f t="shared" ref="N290:R290" si="18">SUM(N286:N289)</f>
+        <v>7</v>
+      </c>
+      <c r="O290" s="1">
+        <f t="shared" si="18"/>
+        <v>10</v>
+      </c>
+      <c r="P290" s="1">
+        <f t="shared" si="18"/>
+        <v>8</v>
+      </c>
+      <c r="R290" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="S290" s="1">
+        <f>SUM(S286:S289)</f>
+        <v>11</v>
+      </c>
+      <c r="T290" s="1">
+        <f>SUM(T286:T289)</f>
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="26">
+    <mergeCell ref="B284:M284"/>
+    <mergeCell ref="A285:A290"/>
+    <mergeCell ref="J285:J290"/>
+    <mergeCell ref="R286:R289"/>
+    <mergeCell ref="J215:J220"/>
+    <mergeCell ref="A215:A220"/>
+    <mergeCell ref="A192:A197"/>
+    <mergeCell ref="A168:A173"/>
+    <mergeCell ref="B191:M191"/>
+    <mergeCell ref="J192:J197"/>
     <mergeCell ref="B261:M261"/>
     <mergeCell ref="A262:A267"/>
     <mergeCell ref="J262:J267"/>
@@ -18356,12 +21468,6 @@
     <mergeCell ref="A238:A243"/>
     <mergeCell ref="J238:J243"/>
     <mergeCell ref="B214:M214"/>
-    <mergeCell ref="J215:J220"/>
-    <mergeCell ref="A215:A220"/>
-    <mergeCell ref="A192:A197"/>
-    <mergeCell ref="A168:A173"/>
-    <mergeCell ref="B191:M191"/>
-    <mergeCell ref="J192:J197"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>